<commit_message>
SOW workload analysis update
</commit_message>
<xml_diff>
--- a/STX2020-SOW-Analysis.xlsx
+++ b/STX2020-SOW-Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Intel\StarlingX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0272331C-2824-47EB-845C-E37AE934763E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4097C2E4-9943-4031-A6B7-9D6F57768079}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="847" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -443,15 +443,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>■ 作业内容理解
-CentOS8 Kernel升级工作。
-■ 目前为止实际工作量
-11月开始合计约1.5人月；
-■ 当前剩余工作内容
-Build Env(dnf)升级/Kernel upgrade，预计约1人月，预计3月份内可以完成；</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>Only Kernel &amp; Driver code</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -479,21 +470,7 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>■ 工作量预估
-(el8 RT 版本内核与el7 RT的详细差异暂时不清楚，按目前了解进行估计)
-Driver：基本可复用STD(SPEC/Code留用、仅做编译及测试)
-Kernel：需重新对应，部分可以参考STD，Patch估计比STD多10个左右
-对于部分SRPM/TAR受RT的影响需要修改，合计预估约6人月；</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>目前需要Python2升级为Python3的包，正在调查中、仅tar包接近52个，srpm包正在调查中，更新的信息已经上传Github。</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>■ 工作量预估
-每个包升级的工作量从4人时～2人周不等。
-平均值约3人日/包、估计约40个包，合计约90人日(4.5人月)。</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -518,6 +495,29 @@
   <si>
     <t>工作量：尚不确定，需要确认升级频度及包的数量确定。
 综合难度考虑约2.5人周/件。</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>■ 作业内容理解
+CentOS8 Kernel升级工作。
+■ 目前为止实际工作量
+11月开始合计约1.5人月；
+■ 当前剩余工作内容
+Build Env(dnf)升级/Kernel upgrade，剩余工作量约1.5人月，预计3月份内可以完成；</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>■ 工作量预估
+(el8 RT 版本内核与el7 RT的详细差异暂时不清楚，按目前了解进行估计)
+Driver：基本可复用STD(SPEC/Code留用、仅做编译及测试)
+Kernel：需重新对应，部分可以参考STD，RT Patch估计比STD多10个左右
+对于部分SRPM/TAR受RT的影响需要修改，合计预估约6人月；</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>■ 工作量预估
+每个包升级的工作量从4人时～2人周不等。
+平均值约3人日/包、估计约50个包，合计约150人日.</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -1945,6 +1945,9 @@
     <xf numFmtId="0" fontId="1" fillId="12" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="177" fontId="1" fillId="12" borderId="61" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1960,6 +1963,15 @@
     <xf numFmtId="0" fontId="9" fillId="13" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1989,18 +2001,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="177" fontId="1" fillId="12" borderId="61" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2864,17 +2864,17 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" s="86" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
-      <c r="B2" s="109" t="s">
+      <c r="B2" s="110" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="109"/>
-      <c r="D2" s="109"/>
-      <c r="E2" s="105" t="s">
+      <c r="C2" s="110"/>
+      <c r="D2" s="110"/>
+      <c r="E2" s="106" t="s">
         <v>33</v>
       </c>
-      <c r="F2" s="106"/>
-      <c r="G2" s="106"/>
-      <c r="H2" s="107"/>
+      <c r="F2" s="107"/>
+      <c r="G2" s="107"/>
+      <c r="H2" s="108"/>
     </row>
     <row r="3" spans="2:9" s="86" customFormat="1" ht="15.75" x14ac:dyDescent="0.15">
       <c r="B3" s="82" t="s">
@@ -2898,56 +2898,56 @@
       </c>
     </row>
     <row r="4" spans="2:9" ht="110.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B4" s="108" t="s">
+      <c r="B4" s="109" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="120" t="s">
+      <c r="C4" s="111" t="s">
         <v>41</v>
       </c>
-      <c r="D4" s="120" t="s">
+      <c r="D4" s="111" t="s">
         <v>47</v>
       </c>
       <c r="E4" s="81" t="s">
         <v>58</v>
       </c>
       <c r="F4" s="99" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="G4" s="91">
         <f>1.5</f>
         <v>1.5</v>
       </c>
       <c r="H4" s="89" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="2:9" ht="128.25" x14ac:dyDescent="0.15">
-      <c r="B5" s="108"/>
-      <c r="C5" s="121"/>
-      <c r="D5" s="121"/>
+      <c r="B5" s="109"/>
+      <c r="C5" s="112"/>
+      <c r="D5" s="112"/>
       <c r="E5" s="81" t="s">
         <v>59</v>
       </c>
       <c r="F5" s="99" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G5" s="91">
         <f>3*4+1.5*6</f>
         <v>21</v>
       </c>
       <c r="H5" s="89" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="2:9" ht="108" x14ac:dyDescent="0.15">
-      <c r="B6" s="108"/>
-      <c r="C6" s="121"/>
-      <c r="D6" s="121"/>
+      <c r="B6" s="109"/>
+      <c r="C6" s="112"/>
+      <c r="D6" s="112"/>
       <c r="E6" s="81" t="s">
         <v>60</v>
       </c>
       <c r="F6" s="98" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G6" s="92">
         <f>1.5</f>
@@ -2958,15 +2958,15 @@
       </c>
       <c r="I6" s="88"/>
     </row>
-    <row r="7" spans="2:9" ht="108" x14ac:dyDescent="0.15">
-      <c r="B7" s="108"/>
-      <c r="C7" s="122"/>
-      <c r="D7" s="122"/>
+    <row r="7" spans="2:9" ht="117" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B7" s="109"/>
+      <c r="C7" s="113"/>
+      <c r="D7" s="113"/>
       <c r="E7" s="81" t="s">
         <v>61</v>
       </c>
       <c r="F7" s="98" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="G7" s="92">
         <f>2*3</f>
@@ -2978,7 +2978,7 @@
       <c r="I7" s="88"/>
     </row>
     <row r="8" spans="2:9" ht="73.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B8" s="108"/>
+      <c r="B8" s="109"/>
       <c r="C8" s="84" t="s">
         <v>40</v>
       </c>
@@ -2989,18 +2989,18 @@
         <v>44</v>
       </c>
       <c r="F8" s="100" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="G8" s="101">
-        <f>3*40/20</f>
-        <v>6</v>
+        <f>3*50/20</f>
+        <v>7.5</v>
       </c>
       <c r="H8" s="102" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="2:9" ht="75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B9" s="108" t="s">
+      <c r="B9" s="109" t="s">
         <v>35</v>
       </c>
       <c r="C9" s="84" t="s">
@@ -3013,18 +3013,18 @@
         <v>44</v>
       </c>
       <c r="F9" s="104" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="G9" s="91">
         <f>(3+1.5*2)/4*10</f>
         <v>15</v>
       </c>
       <c r="H9" s="81" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="2:9" ht="71.25" x14ac:dyDescent="0.15">
-      <c r="B10" s="108"/>
+      <c r="B10" s="109"/>
       <c r="C10" s="84" t="s">
         <v>38</v>
       </c>
@@ -3042,24 +3042,24 @@
         <v>12.5</v>
       </c>
       <c r="H10" s="90" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="2:9" ht="31.5" x14ac:dyDescent="0.15">
-      <c r="B11" s="108"/>
+      <c r="B11" s="109"/>
       <c r="C11" s="84" t="s">
         <v>37</v>
       </c>
       <c r="D11" s="85"/>
       <c r="E11" s="90"/>
       <c r="F11" s="98" t="s">
-        <v>74</v>
-      </c>
-      <c r="G11" s="123" t="s">
-        <v>73</v>
+        <v>71</v>
+      </c>
+      <c r="G11" s="105" t="s">
+        <v>70</v>
       </c>
       <c r="H11" s="103" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="2:9" ht="47.25" x14ac:dyDescent="0.15">
@@ -3090,7 +3090,7 @@
       </c>
       <c r="G14" s="94">
         <f>SUM(G4:G12)</f>
-        <v>68.5</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.15">
@@ -3099,7 +3099,7 @@
       </c>
       <c r="G15" s="96">
         <f>G14/10</f>
-        <v>6.85</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -3136,126 +3136,126 @@
   <sheetData>
     <row r="1" spans="2:103" ht="14.25" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:103" ht="19.5" thickTop="1" x14ac:dyDescent="0.15">
-      <c r="B2" s="110" t="s">
+      <c r="B2" s="114" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="111"/>
-      <c r="D2" s="111"/>
-      <c r="E2" s="111"/>
-      <c r="F2" s="111"/>
-      <c r="G2" s="111"/>
-      <c r="H2" s="111"/>
-      <c r="I2" s="111"/>
-      <c r="J2" s="112"/>
-      <c r="L2" s="116" t="s">
+      <c r="C2" s="115"/>
+      <c r="D2" s="115"/>
+      <c r="E2" s="115"/>
+      <c r="F2" s="115"/>
+      <c r="G2" s="115"/>
+      <c r="H2" s="115"/>
+      <c r="I2" s="115"/>
+      <c r="J2" s="116"/>
+      <c r="L2" s="120" t="s">
         <v>1</v>
       </c>
-      <c r="M2" s="117"/>
-      <c r="N2" s="117"/>
-      <c r="O2" s="117"/>
-      <c r="P2" s="117"/>
-      <c r="Q2" s="117"/>
-      <c r="R2" s="117"/>
-      <c r="S2" s="117"/>
-      <c r="T2" s="117"/>
-      <c r="U2" s="117"/>
-      <c r="V2" s="117"/>
-      <c r="W2" s="117"/>
-      <c r="X2" s="117"/>
-      <c r="Y2" s="117"/>
-      <c r="Z2" s="117"/>
-      <c r="AA2" s="117"/>
-      <c r="AB2" s="117"/>
-      <c r="AC2" s="117"/>
-      <c r="AD2" s="117"/>
-      <c r="AE2" s="117"/>
-      <c r="AF2" s="117"/>
-      <c r="AG2" s="117"/>
-      <c r="AH2" s="117"/>
-      <c r="AI2" s="117"/>
-      <c r="AJ2" s="117"/>
-      <c r="AK2" s="117"/>
-      <c r="AL2" s="117"/>
-      <c r="AM2" s="117"/>
-      <c r="AN2" s="117"/>
-      <c r="AO2" s="117"/>
-      <c r="AP2" s="118" t="s">
+      <c r="M2" s="121"/>
+      <c r="N2" s="121"/>
+      <c r="O2" s="121"/>
+      <c r="P2" s="121"/>
+      <c r="Q2" s="121"/>
+      <c r="R2" s="121"/>
+      <c r="S2" s="121"/>
+      <c r="T2" s="121"/>
+      <c r="U2" s="121"/>
+      <c r="V2" s="121"/>
+      <c r="W2" s="121"/>
+      <c r="X2" s="121"/>
+      <c r="Y2" s="121"/>
+      <c r="Z2" s="121"/>
+      <c r="AA2" s="121"/>
+      <c r="AB2" s="121"/>
+      <c r="AC2" s="121"/>
+      <c r="AD2" s="121"/>
+      <c r="AE2" s="121"/>
+      <c r="AF2" s="121"/>
+      <c r="AG2" s="121"/>
+      <c r="AH2" s="121"/>
+      <c r="AI2" s="121"/>
+      <c r="AJ2" s="121"/>
+      <c r="AK2" s="121"/>
+      <c r="AL2" s="121"/>
+      <c r="AM2" s="121"/>
+      <c r="AN2" s="121"/>
+      <c r="AO2" s="121"/>
+      <c r="AP2" s="122" t="s">
         <v>2</v>
       </c>
-      <c r="AQ2" s="118"/>
-      <c r="AR2" s="118"/>
-      <c r="AS2" s="118"/>
-      <c r="AT2" s="118"/>
-      <c r="AU2" s="118"/>
-      <c r="AV2" s="118"/>
-      <c r="AW2" s="118"/>
-      <c r="AX2" s="118"/>
-      <c r="AY2" s="118"/>
-      <c r="AZ2" s="118"/>
-      <c r="BA2" s="118"/>
-      <c r="BB2" s="118"/>
-      <c r="BC2" s="118"/>
-      <c r="BD2" s="118"/>
-      <c r="BE2" s="118"/>
-      <c r="BF2" s="118"/>
-      <c r="BG2" s="118"/>
-      <c r="BH2" s="118"/>
-      <c r="BI2" s="118"/>
-      <c r="BJ2" s="118"/>
-      <c r="BK2" s="118"/>
-      <c r="BL2" s="118"/>
-      <c r="BM2" s="118"/>
-      <c r="BN2" s="118"/>
-      <c r="BO2" s="118"/>
-      <c r="BP2" s="118"/>
-      <c r="BQ2" s="118"/>
-      <c r="BR2" s="118"/>
-      <c r="BS2" s="118"/>
-      <c r="BT2" s="118"/>
-      <c r="BU2" s="119" t="s">
+      <c r="AQ2" s="122"/>
+      <c r="AR2" s="122"/>
+      <c r="AS2" s="122"/>
+      <c r="AT2" s="122"/>
+      <c r="AU2" s="122"/>
+      <c r="AV2" s="122"/>
+      <c r="AW2" s="122"/>
+      <c r="AX2" s="122"/>
+      <c r="AY2" s="122"/>
+      <c r="AZ2" s="122"/>
+      <c r="BA2" s="122"/>
+      <c r="BB2" s="122"/>
+      <c r="BC2" s="122"/>
+      <c r="BD2" s="122"/>
+      <c r="BE2" s="122"/>
+      <c r="BF2" s="122"/>
+      <c r="BG2" s="122"/>
+      <c r="BH2" s="122"/>
+      <c r="BI2" s="122"/>
+      <c r="BJ2" s="122"/>
+      <c r="BK2" s="122"/>
+      <c r="BL2" s="122"/>
+      <c r="BM2" s="122"/>
+      <c r="BN2" s="122"/>
+      <c r="BO2" s="122"/>
+      <c r="BP2" s="122"/>
+      <c r="BQ2" s="122"/>
+      <c r="BR2" s="122"/>
+      <c r="BS2" s="122"/>
+      <c r="BT2" s="122"/>
+      <c r="BU2" s="123" t="s">
         <v>3</v>
       </c>
-      <c r="BV2" s="119"/>
-      <c r="BW2" s="119"/>
-      <c r="BX2" s="119"/>
-      <c r="BY2" s="119"/>
-      <c r="BZ2" s="119"/>
-      <c r="CA2" s="119"/>
-      <c r="CB2" s="119"/>
-      <c r="CC2" s="119"/>
-      <c r="CD2" s="119"/>
-      <c r="CE2" s="119"/>
-      <c r="CF2" s="119"/>
-      <c r="CG2" s="119"/>
-      <c r="CH2" s="119"/>
-      <c r="CI2" s="119"/>
-      <c r="CJ2" s="119"/>
-      <c r="CK2" s="119"/>
-      <c r="CL2" s="119"/>
-      <c r="CM2" s="119"/>
-      <c r="CN2" s="119"/>
-      <c r="CO2" s="119"/>
-      <c r="CP2" s="119"/>
-      <c r="CQ2" s="119"/>
-      <c r="CR2" s="119"/>
-      <c r="CS2" s="119"/>
-      <c r="CT2" s="119"/>
-      <c r="CU2" s="119"/>
-      <c r="CV2" s="119"/>
-      <c r="CW2" s="119"/>
-      <c r="CX2" s="119"/>
-      <c r="CY2" s="119"/>
+      <c r="BV2" s="123"/>
+      <c r="BW2" s="123"/>
+      <c r="BX2" s="123"/>
+      <c r="BY2" s="123"/>
+      <c r="BZ2" s="123"/>
+      <c r="CA2" s="123"/>
+      <c r="CB2" s="123"/>
+      <c r="CC2" s="123"/>
+      <c r="CD2" s="123"/>
+      <c r="CE2" s="123"/>
+      <c r="CF2" s="123"/>
+      <c r="CG2" s="123"/>
+      <c r="CH2" s="123"/>
+      <c r="CI2" s="123"/>
+      <c r="CJ2" s="123"/>
+      <c r="CK2" s="123"/>
+      <c r="CL2" s="123"/>
+      <c r="CM2" s="123"/>
+      <c r="CN2" s="123"/>
+      <c r="CO2" s="123"/>
+      <c r="CP2" s="123"/>
+      <c r="CQ2" s="123"/>
+      <c r="CR2" s="123"/>
+      <c r="CS2" s="123"/>
+      <c r="CT2" s="123"/>
+      <c r="CU2" s="123"/>
+      <c r="CV2" s="123"/>
+      <c r="CW2" s="123"/>
+      <c r="CX2" s="123"/>
+      <c r="CY2" s="123"/>
     </row>
     <row r="3" spans="2:103" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="113"/>
-      <c r="C3" s="114"/>
-      <c r="D3" s="114"/>
-      <c r="E3" s="114"/>
-      <c r="F3" s="114"/>
-      <c r="G3" s="114"/>
-      <c r="H3" s="114"/>
-      <c r="I3" s="114"/>
-      <c r="J3" s="115"/>
+      <c r="B3" s="117"/>
+      <c r="C3" s="118"/>
+      <c r="D3" s="118"/>
+      <c r="E3" s="118"/>
+      <c r="F3" s="118"/>
+      <c r="G3" s="118"/>
+      <c r="H3" s="118"/>
+      <c r="I3" s="118"/>
+      <c r="J3" s="119"/>
       <c r="L3" s="74">
         <v>43770</v>
       </c>

</xml_diff>